<commit_message>
fix centered on qrcode
</commit_message>
<xml_diff>
--- a/bot/shablon.xlsx
+++ b/bot/shablon.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28821"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alfatech.uz\Documents\telegram_bot\autoprinter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alfatech.uz\Documents\nakladnoy_printer\bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EBFB06-1BF0-441F-9777-5A6169461313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72535112-B269-4958-B795-5FB4EDB11DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,55 +178,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>466724</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>209969</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2238375</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30440020-5951-75A5-063D-40A760AACB59}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1895474" y="400469"/>
-          <a:ext cx="1771651" cy="1056856"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -532,7 +483,7 @@
   <dimension ref="A2:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:F5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -665,6 +616,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:F4"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A5:C5"/>
@@ -673,15 +630,8 @@
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:F4"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="94" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>